<commit_message>
Include db context and and other files
</commit_message>
<xml_diff>
--- a/Analyzer/Documents/DB.xlsx
+++ b/Analyzer/Documents/DB.xlsx
@@ -16,12 +16,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>table per stock</t>
   </si>
   <si>
     <t>table per data figure like eps</t>
+  </si>
+  <si>
+    <t>StockName</t>
+  </si>
+  <si>
+    <t>Price Table</t>
+  </si>
+  <si>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>OID</t>
   </si>
 </sst>
 </file>
@@ -353,22 +365,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>